<commit_message>
added configuration for extent report. Renamed and moved log4j2.xml to classpath
</commit_message>
<xml_diff>
--- a/src/main/java/resources/TestData.xlsx
+++ b/src/main/java/resources/TestData.xlsx
@@ -5,27 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkapadia\eclipse-workspace\Expedia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkapadia\eclipse-workspace\Expedia\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF41E0E-8ECE-4417-9EB4-FE4F1154D27F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF222B2-9DBD-4554-9240-0D6780C3B6FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
   <si>
     <t>Destination</t>
   </si>
@@ -40,6 +46,27 @@
   </si>
   <si>
     <t>Connecticut</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>TC_Description</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Status (Pass/Fail)</t>
+  </si>
+  <si>
+    <t>Enter checkin date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to expedia.com
+Click on check-in input field
+Enter date
+</t>
   </si>
 </sst>
 </file>
@@ -48,7 +75,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -75,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,15 +110,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,20 +420,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -396,7 +445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -405,6 +454,228 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>7</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>